<commit_message>
SQL tables for class updated in 2NF
</commit_message>
<xml_diff>
--- a/Week11Notes/SQLDay1Tables.xlsx
+++ b/Week11Notes/SQLDay1Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Skillstorm\JavaVettecLessons\Week11Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BF0545-CE45-4845-9876-3B66D69C5FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA685E1-E9DE-4517-8803-A5A452787A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25455" yWindow="1440" windowWidth="20565" windowHeight="11910" activeTab="1" xr2:uid="{08E80810-BA5D-4DD5-A02D-76D96DC358BE}"/>
+    <workbookView xWindow="-11664" yWindow="12852" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{08E80810-BA5D-4DD5-A02D-76D96DC358BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="294">
   <si>
     <t>Warehouse</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Trumpet</t>
   </si>
   <si>
-    <t>LocationName</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Airline</t>
-  </si>
-  <si>
     <t>Packages</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>Pittsburg</t>
   </si>
   <si>
-    <t>Pittsburgh</t>
-  </si>
-  <si>
     <t>Egypt</t>
   </si>
   <si>
@@ -584,9 +575,6 @@
     <t>&lt; This columns forms the relationship between our tables</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
@@ -599,15 +587,9 @@
     <t>Job (FK)</t>
   </si>
   <si>
-    <t>SamuraiId</t>
-  </si>
-  <si>
     <t>FollowsCode</t>
   </si>
   <si>
-    <t>Weapon</t>
-  </si>
-  <si>
     <t>Armor</t>
   </si>
   <si>
@@ -620,15 +602,9 @@
     <t>SkillLevel</t>
   </si>
   <si>
-    <t>BattleId</t>
-  </si>
-  <si>
     <t>Terrain</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Weather</t>
   </si>
   <si>
@@ -752,15 +728,6 @@
     <t>Cors</t>
   </si>
   <si>
-    <t>LanguageId</t>
-  </si>
-  <si>
-    <t>LocationId</t>
-  </si>
-  <si>
-    <t>AttractionId</t>
-  </si>
-  <si>
     <t>Beaches</t>
   </si>
   <si>
@@ -792,6 +759,174 @@
   </si>
   <si>
     <t>LocationAttractions</t>
+  </si>
+  <si>
+    <t>ProductId(FK)</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>&lt; Shipments</t>
+  </si>
+  <si>
+    <t>ShippingNumber(PK)</t>
+  </si>
+  <si>
+    <t>&lt;Inventory</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>LanguageId(PK)</t>
+  </si>
+  <si>
+    <t>LocationId(FK)</t>
+  </si>
+  <si>
+    <t>LanguageId(FK)</t>
+  </si>
+  <si>
+    <t>AttractionId(PK)</t>
+  </si>
+  <si>
+    <t>AttractionId(FK)</t>
+  </si>
+  <si>
+    <t>ConfirmationNumber(PK)</t>
+  </si>
+  <si>
+    <t>AirlineId(FK)</t>
+  </si>
+  <si>
+    <t>Package(FK)</t>
+  </si>
+  <si>
+    <t>&lt; Trips</t>
+  </si>
+  <si>
+    <t>AirlineId(PK)</t>
+  </si>
+  <si>
+    <t>Airlines</t>
+  </si>
+  <si>
+    <t>PackageId(PK)</t>
+  </si>
+  <si>
+    <t>Location(FK)</t>
+  </si>
+  <si>
+    <t>&gt; airlines</t>
+  </si>
+  <si>
+    <t>&gt; destinations</t>
+  </si>
+  <si>
+    <t>&gt; packages</t>
+  </si>
+  <si>
+    <t>&lt; Movies</t>
+  </si>
+  <si>
+    <t>Companies</t>
+  </si>
+  <si>
+    <t>CompanyId</t>
+  </si>
+  <si>
+    <t>Skillstorm</t>
+  </si>
+  <si>
+    <t>Justice League</t>
+  </si>
+  <si>
+    <t>Rebellion</t>
+  </si>
+  <si>
+    <t>&lt; positions</t>
+  </si>
+  <si>
+    <t>PositionCompanies</t>
+  </si>
+  <si>
+    <t>PositionId(FK)</t>
+  </si>
+  <si>
+    <t>CompanyId(FK)</t>
+  </si>
+  <si>
+    <t>Weapons</t>
+  </si>
+  <si>
+    <t>Bow</t>
+  </si>
+  <si>
+    <t>SamuraiWeapons</t>
+  </si>
+  <si>
+    <t>&lt;Samurai</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Armor(FK)</t>
+  </si>
+  <si>
+    <t>WeaponId(PK)</t>
+  </si>
+  <si>
+    <t>SamuraiId(PK)</t>
+  </si>
+  <si>
+    <t>SamuraiId(FK)</t>
+  </si>
+  <si>
+    <t>WeaponId(FK)</t>
+  </si>
+  <si>
+    <t>ArmorId(PK)</t>
+  </si>
+  <si>
+    <t>BattleId(PK)</t>
+  </si>
+  <si>
+    <t>Landmarks</t>
+  </si>
+  <si>
+    <t>LandmarkId(PK)</t>
+  </si>
+  <si>
+    <t>WeatherId</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Weather(FK)</t>
   </si>
 </sst>
 </file>
@@ -810,15 +945,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -846,11 +987,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -860,13 +1023,270 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -917,74 +1337,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1163,15 +1515,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>373140</xdr:colOff>
+      <xdr:colOff>87488</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>835740</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:colOff>623326</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3706</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
@@ -1187,9 +1539,9 @@
             <xdr14:cNvContentPartPr/>
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="4602240" y="1184760"/>
-            <a:ext cx="462600" cy="447120"/>
+          <xdr14:xfrm rot="15597417">
+            <a:off x="5035621" y="2053168"/>
+            <a:ext cx="562506" cy="535838"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -1212,9 +1564,9 @@
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4593600" y="1175760"/>
-              <a:ext cx="480240" cy="464760"/>
+            <a:xfrm rot="15597417">
+              <a:off x="5026855" y="2044171"/>
+              <a:ext cx="580404" cy="553471"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1233,8 +1585,8 @@
       <xdr:rowOff>136800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>23160</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>990900</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
@@ -1552,25 +1904,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1253580</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>397934</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3132</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>937680</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1099486</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>50799</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="17" name="Ink 16">
+            <xdr14:cNvPr id="22" name="Ink 21">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C59091E8-2AA1-194F-533E-C4A0C53AE8F1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FBB8FC9-39D5-3D60-B850-1E6C8FE87C19}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1578,18 +1930,18 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="10984320" y="943200"/>
-            <a:ext cx="941400" cy="672120"/>
+            <a:off x="4250267" y="375665"/>
+            <a:ext cx="7034619" cy="1351534"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
       <mc:Fallback>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="17" name="Ink 16">
+            <xdr:cNvPr id="22" name="Ink 21">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C59091E8-2AA1-194F-533E-C4A0C53AE8F1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FBB8FC9-39D5-3D60-B850-1E6C8FE87C19}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1603,8 +1955,8 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10975680" y="934560"/>
-              <a:ext cx="959040" cy="689760"/>
+              <a:off x="4241627" y="367027"/>
+              <a:ext cx="7052259" cy="1369171"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1670,9 +2022,9 @@
       <inkml:brushProperty name="color" value="#FFC114"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">128 1175 24575,'53'-44'0,"-39"35"0,-2-1 0,0 0 0,13-13 0,23-20 0,-40 37 0,1-1 0,-1 0 0,0-1 0,0 1 0,12-18 0,-5 3 0,1 2 0,33-33 0,16-19 0,-48 52 0,37-35 0,-6 8 0,-38 35 0,-1 0 0,15-27 0,11-13 0,35-44 0,-54 74 0,-1-1 0,-2 0 0,0-1 0,10-26 0,22-43 0,-36 76 0,-1 0 0,7-21 0,2-8 0,-7 14-1365,-7 17-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1503.56">551 138 24575,'12'-1'0,"1"-1"0,0 0 0,-1 0 0,0-1 0,20-8 0,-18 6 0,1 0 0,1 1 0,16-2 0,-16 3 0,-1 0 0,1-1 0,24-10 0,21-6 0,106-22 0,-147 38 0,-14 2 0,1 1 0,0-1 0,0 1 0,1 1 0,-1-1 0,9 2 0,-14-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,2 4 0,2 11 0,0-1 0,3 20 0,9 29 0,0 2 0,-15-50 0,2-1 0,8 24 0,40 116-1365,-47-143-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3273.17">1 858 24575,'1'13'0,"1"0"0,0 0 0,1 0 0,1-1 0,0 1 0,12 23 0,8 29 0,-17-44 0,2 0 0,1-1 0,0 0 0,22 31 0,-21-33 0,-9-15 0,1 1 0,0 0 0,-1-1 0,1 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0-1 0,0 0 0,0 0 0,0 0 0,6 2 0,1-2 0,0 0 0,0-1 0,1 0 0,-1 0 0,12-2 0,402-1-1365,-407 2-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">153 1408 24575,'64'-52'0,"-48"41"0,-1-1 0,0 0 0,14-16 0,29-23 0,-48 43 0,0 0 0,0 0 0,-1-1 0,1-1 0,14-20 0,-6 5 0,1 0 0,40-39 0,18-21 0,-56 60 0,44-41 0,-8 10 0,-45 42 0,-1-1 0,18-31 0,12-17 0,44-52 0,-66 89 0,-1-1 0,-2-2 0,-1 1 0,12-32 0,28-51 0,-44 91 0,-2-1 0,8-25 0,5-9 0,-11 17-1365,-7 20-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1503.56">660 165 24575,'15'-1'0,"0"-1"0,0 0 0,0-1 0,0-1 0,23-9 0,-21 7 0,1 0 0,0 2 0,22-4 0,-22 5 0,1-1 0,-1-1 0,31-12 0,24-6 0,127-28 0,-177 46 0,-15 3 0,1 0 0,-1 1 0,1 0 0,-1 0 0,1 0 0,10 2 0,-17-1 0,1 1 0,0 0 0,0-1 0,-1 1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1 4 0,5 13 0,-1 0 0,4 22 0,10 36 0,0 3 0,-17-62 0,1 1 0,11 28 0,48 139-1365,-58-171-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3273.17">1 1028 24575,'1'16'0,"2"-1"0,0 1 0,0-1 0,2 0 0,-1 0 0,15 28 0,10 35 0,-20-53 0,2 0 0,0 0 0,2-1 0,25 37 0,-25-40 0,-10-16 0,0-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0-1 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 0 0,7 3 0,1-3 0,1 1 0,-1-2 0,0 0 0,1 0 0,13-2 0,482-2-1365,-487 3-5461</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1832,7 +2184,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2023-05-16T15:59:06.848"/>
+      <inkml:timestamp xml:id="ts0" timeString="2023-05-17T14:23:40.827"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.05" units="cm"/>
@@ -1840,29 +2192,106 @@
       <inkml:brushProperty name="color" value="#FFC114"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2191 1867 24575,'-4'-1'0,"0"1"0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-4-3 0,-34-29 0,30 24 0,-116-100 0,-56-34 0,157 122 0,-27-31 0,33 31 0,-1 2 0,-27-22 0,-42-31 0,1-1 0,57 45 0,-9-6 0,37 31 0,-1 1 0,1-1 0,0 0 0,0 0 0,1-1 0,-6-7 0,6 8 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,-8-6 0,-8-4 0,0-2 0,-20-18 0,-25-18 0,35 30 0,-28-28 0,-16-12 0,42 36 0,-25-15 0,39 27 0,0 1 0,2-2 0,-22-21 0,17 15 0,-71-57 0,91 76 0,-39-28 0,-58-53 0,-73-89 0,134 140 0,27 23 0,0 0 0,1 0 0,-14-16 0,17 18-227,0 0-1,0 0 1,0 1-1,-1-1 1,-8-4-1,4 3-6598</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1663.93">116 851 24575,'2'-3'0,"0"0"0,0 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,0-5 0,1-50 0,-2 42 0,-2-17 0,-10-63 0,3 36 0,6 48 0,0 1 0,0-1 0,-1 1 0,-1 0 0,-8-17 0,7 19 0,1 0 0,1-1 0,0 1 0,1-1 0,-1 0 0,2 0 0,-2-15 0,1 1 0,0 0 0,-2 0 0,-14-42 0,15 53 0,1-2 0,0 0 0,0 0 0,1-25 0,-3-22 0,4 62 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,2-1 0,-1 1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0 0 0,4 0 0,0 0 0,1 0 0,-1 1 0,0 0 0,1 1 0,-1 0 0,0 0 0,8 4 0,19 10 0,1-2 0,60 17 0,-91-30 0,60 20 0,76 33 0,-116-45 0,0-2 0,0 0 0,1-2 0,29 3 0,-36-5 0,91 14 0,-3 4 0,-91-18 13,1-1 0,25 0 0,-31-2-153,-1 0-1,1 0 1,0 1-1,0 0 1,-1 1 0,1 0-1,-1 1 1,0 0-1,16 7 1,-14-3-6686</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8306.74">1556 1761 24575,'488'0'0,"-468"1"0,0 1 0,27 6 0,-25-4 0,38 3 0,-45-6 0,10-1 0,-1 1 0,47 9 0,-37-1 0,-10-3 0,-1-1 0,2 0 0,29 1 0,-43-6 0,0 1 0,-1 1 0,1 0 0,11 4 0,-22-6 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,-1-29 0,2 24 0,-5-50 0,6-103 0,19 52 0,-19 105-52,-2-1-49,2 0 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,4-5 0,4-1-6725</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">19330 3467 24575,'-8'-2'0,"0"1"0,0-2 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1-1 0,1 0 0,-12-9 0,-18-10 0,-28-8 210,-449-196-2753,245 123-416,111 40 2378,-225-58 1,-60-12 353,95 24-73,181 56 736,-40-10 165,-44-11-726,28 7 18,-157-6 1444,181 25 3396,-77 16-4628,134 29-105,57 3 0,-88-12 0,-34-17-920,-66-8 920,122 35 0,101 4 0,-1-2 0,-54-9 0,-138-31 767,97 23-690,-201 2-1,300 13-76,0-1 0,-79-18 0,80 12 0,0 2 0,-84-4 0,75 11 0,-1-3 0,1-2 0,0-3 0,0-2 0,-72-25 0,103 30 0,0 1 0,0 1 0,-42-2 0,42 5 0,1-1 0,0-1 0,0-2 0,-33-9 0,26 5 0,-1 1 0,1 2 0,-35-3 0,-40-8 0,-63-12 0,92 14 0,-139-11 0,182 21 0,1 0 0,-42-13 0,46 10 0,0 1 0,0 1 0,-45-2 0,45 6 0,-47-10 0,-18-1 0,36 7 0,0-2 0,-74-22 0,82 17 0,-1 2 0,0 2 0,-82-3 0,73 9-162,0-3-1,-63-14 0,60 9-62,-103-6 1,115 13 141,1-2-1,0-3 1,-57-16 0,56 12-21,0 2-1,-93-8 1,71 13 605,1-4 0,-132-35 0,149 31-421,25 9-80,0 1 0,0 2 0,-52 1 0,50 2 0,0-1 0,0-2 0,-38-6 0,15-2 0,-106-2 0,-9-2 0,117 9 0,-81 2 0,-9 0 0,-28-26 0,69 14 0,71 10 0,-1 0 0,-33 0 0,-90-10 0,104 9 0,-60-2 0,53 9 0,16 0 0,1-1 0,0-2 0,-77-14 0,-81-13 0,146 21 0,1 2 0,-1 3 0,-94 6 0,31 0 0,88-3 0,0-2 0,0 0 0,-46-11 0,-30-11 0,-1 4 0,-132-6 0,165 23 0,23 3 0,-89-15 0,82 8 0,-1 2 0,-90 3 0,90 3 0,0-2 0,-87-13 0,47-3 0,-2 5 0,-106-1 0,159 13 0,0-2 0,-63-12 0,-45-16 0,109 22 0,0 3 0,0 1 0,0 3 0,-60 5 0,-2-1 0,46-6-132,0-3 0,0-2 0,1-3 0,-89-28 0,97 27 132,0 3 0,-66-4 0,-27-4 0,35-4 139,56 9 35,0 2-1,-101-4 1,122 12-174,-60-10 0,58 6 0,-54-2 0,-1020 9 0,1086-2 0,1-1 0,-38-10 0,36 7 0,0 1 0,-27-1 0,-434 5 0,466 2 0,0 0 0,0 1 0,0 1 0,0 0 0,-21 9 0,27-8 0,0 0 0,0-1 0,0-1 0,-1 0 0,1-1 0,-1 0 0,1-1 0,-1 0 0,0-1 0,1 0 0,-1-1 0,-20-5 0,-23-16-1365,31 12-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1148.5">859 1 24575,'-4'1'0,"1"0"0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,-5 4 0,-13 8 0,-124 46 0,65-30 0,48-20 0,1 2 0,-30 17 0,58-28 0,-21 14 0,-1-2 0,0 0 0,-1-2 0,-1-1 0,1 0 0,-35 5 0,54-13 0,0 0 0,0 1 0,-1 0 0,1 0 0,1 0 0,-1 1 0,1 0 0,-1 1 0,-6 6 0,6-6 0,0 0 0,0 0 0,0 0 0,0-1 0,0 0 0,-1-1 0,-14 5 0,17-7 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-8 7 0,10-6 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,0 0 0,1-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 8 0,-1 7 0,2 0 0,0 0 0,5 38 0,-4-49 0,1 0 0,0 0 0,0 0 0,1 0 0,0-1 0,1 0 0,0 1 0,0-1 0,0 0 0,1-1 0,10 13 0,-6-8 0,-1 0 0,0 1 0,-1 0 0,0 0 0,-1 1 0,0 0 0,5 21 0,-5-19 0,-1 1 0,2-1 0,0 0 0,1-1 0,12 19 0,3-1 0,28 53 0,-25-41 0,25 48 0,21 23 0,-51-80 0,0 0 0,34 40 0,-54-74-62,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1-1 0,1 1-1,0-1 1,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1-1 0,1 1 0,3-1 0,11-1-6764</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2816.93">18761 2600 24575,'9'0'0,"1"1"0,-1-1 0,0 2 0,1-1 0,-1 1 0,0 1 0,0-1 0,0 2 0,-1-1 0,1 1 0,-1 1 0,0-1 0,0 1 0,0 1 0,-1 0 0,0 0 0,0 0 0,0 1 0,-1 0 0,8 10 0,37 37 0,-40-44 0,0 1 0,-1 0 0,13 17 0,-1 1 0,35 37 0,-42-50 0,0 1 0,0 0 0,-2 1 0,0 0 0,-1 1 0,18 40 0,12 25 0,-30-65 0,-2 0 0,14 36 0,29 57 0,-46-97 0,0-1 0,2 0 0,-1 0 0,16 18 0,14 23 0,-12-16 0,13 27 0,-38-66 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-2 1 0,-28 12 0,-43-9 0,67-4 0,-46 0 0,1 2 0,-57 10 0,-85 7-427,47-8 148,-18 2 566,-203-12 0,164-3-155,110 0-132,-103 4 0,184 0 22,1 1 0,-1 0 0,0 0 0,1 1 0,-17 9 0,-34 10-1519,42-18-5329</inkml:trace>
 </inkml:ink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{169FFBAD-0715-443B-B4F3-FACA77A88672}" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0">
-  <autoFilter ref="A1:G9" xr:uid="{169FFBAD-0715-443B-B4F3-FACA77A88672}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D50E8F65-1B55-4C5F-8B59-411A34969A3A}" name="ProductId (PK)" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{2CD6D77C-265A-4EA7-9C6C-E63277E7F430}" name="Warehouse" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{A21BDBD0-725F-4A29-BDFC-E543B1D57B44}" name="Destination" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{1037C770-5A2C-4AD9-AEC8-0DB53C11560F}" name="ProductType" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{7F33EFD7-1DF3-4672-97C1-F31498422CB4}" name="LabelCreated" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{70274EED-EE35-4CDC-A230-3C47F6ED1C3D}" name="Handler" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{44B3FDF9-24B1-4511-9456-F62C55BD99C2}" name="LastHandled" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{169FFBAD-0715-443B-B4F3-FACA77A88672}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0">
+  <autoFilter ref="A1:D9" xr:uid="{169FFBAD-0715-443B-B4F3-FACA77A88672}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{D50E8F65-1B55-4C5F-8B59-411A34969A3A}" name="ProductId (PK)" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{2CD6D77C-265A-4EA7-9C6C-E63277E7F430}" name="Warehouse" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{1037C770-5A2C-4AD9-AEC8-0DB53C11560F}" name="ProductType" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{44B3FDF9-24B1-4511-9456-F62C55BD99C2}" name="Stock" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{D666F794-0946-4A5B-9BAE-0F3A242BE3B1}" name="Table17" displayName="Table17" ref="L22:M27" totalsRowShown="0">
+  <autoFilter ref="L22:M27" xr:uid="{D666F794-0946-4A5B-9BAE-0F3A242BE3B1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4A515555-28CE-4739-B851-59030A0D992E}" name="PackageId(PK)" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{CB99D568-7B49-4FB6-87F8-F0B64371FA6F}" name="Name" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9B1458FE-FA91-42BC-871C-630EB8E60412}" name="Table3" displayName="Table3" ref="A1:H9" totalsRowShown="0">
+  <autoFilter ref="A1:H9" xr:uid="{9B1458FE-FA91-42BC-871C-630EB8E60412}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{45BFCCB0-CFBB-4B57-8C28-AAC046F29FE2}" name="Title (PK)" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{D78FEB3F-9FBE-4352-BE7A-99B63B84046A}" name="ReleaseYear (PK)" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{D1A66C44-7E6F-4C4D-989B-89C81FC74AFD}" name="Genre" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{BBD5306B-D5DE-44D7-8410-6993F6B3F577}" name="Rating" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{952CD790-64DB-4FBD-BD46-21A5C343B1C9}" name="GrossProfit" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{1C33DB9A-FD12-47A9-AD86-D05FD166765F}" name="Cost" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{2E5F3783-24D8-4EA6-BAF7-DD66ACFB5965}" name="Runtime" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{572EC56E-E2A4-4FC3-9BB8-EC58E78E08A8}" name="ReviewScore"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{608619DC-1C9C-47A5-9711-DDF52ABEDA2F}" name="Table4" displayName="Table4" ref="A1:H8" totalsRowShown="0">
+  <autoFilter ref="A1:H8" xr:uid="{608619DC-1C9C-47A5-9711-DDF52ABEDA2F}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{5A22A79B-FFD4-4DEB-9DBE-192986B98DE1}" name="PersonId (PK)"/>
+    <tableColumn id="2" xr3:uid="{FA34B470-FF1F-4B26-85CD-BCB40CADD0CC}" name="First"/>
+    <tableColumn id="3" xr3:uid="{146CC122-E9F9-442D-B20C-41BFF1898970}" name="Last"/>
+    <tableColumn id="4" xr3:uid="{1333BF0F-E4B6-4F51-B4B5-EA53C991A40F}" name="HairColor"/>
+    <tableColumn id="5" xr3:uid="{6AB9EFF3-157F-4350-BADB-555E7C3890A8}" name="Birthday" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{1D1456BC-3D5F-4581-9CFC-F74BFF30E53B}" name="BloodType"/>
+    <tableColumn id="7" xr3:uid="{B3996C23-B66E-4A7A-BE9F-1DC3E2A16BD0}" name="FirstLanguage"/>
+    <tableColumn id="8" xr3:uid="{5443F791-ACE7-4711-9651-CBBFDC16C2D7}" name="Job (FK)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B2843E5E-9CA7-4DEB-84C1-8D646C92F38C}" name="Table6" displayName="Table6" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{B2843E5E-9CA7-4DEB-84C1-8D646C92F38C}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E5CDF23F-8C1B-4148-9AEA-983FEA37C18D}" name="JobId (PK)"/>
+    <tableColumn id="2" xr3:uid="{9D7E6A9E-2E69-451B-A0FA-E94F9C3676DC}" name="Title"/>
+    <tableColumn id="4" xr3:uid="{305ACE71-C1F4-4890-B6D6-E6F3B884C79B}" name="Salary"/>
+    <tableColumn id="5" xr3:uid="{0337C2FC-F46F-48C4-93E6-0DD9851D869D}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{6CA3EA81-54D9-4B7A-8D09-02F31CB56EDF}" name="Table19" displayName="Table19" ref="A11:B15" totalsRowShown="0">
+  <autoFilter ref="A11:B15" xr:uid="{6CA3EA81-54D9-4B7A-8D09-02F31CB56EDF}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E46F0538-17A7-4690-A35F-2D7286D34FB0}" name="CompanyId"/>
+    <tableColumn id="2" xr3:uid="{AC85D16E-4CCA-447C-8688-96476F0175CE}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{72F50449-5101-422B-AB63-DC6304EDFB5E}" name="Table20" displayName="Table20" ref="D11:E17" totalsRowShown="0">
+  <autoFilter ref="D11:E17" xr:uid="{72F50449-5101-422B-AB63-DC6304EDFB5E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{81EA14AD-8DCF-468B-B44A-FDEFDDA74D9E}" name="PositionId(FK)"/>
+    <tableColumn id="2" xr3:uid="{42AC35F0-737B-48EF-90E0-73A012E31521}" name="CompanyId(FK)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9B4D5B3D-846B-46CC-8CF1-243527D6D766}" name="Table5" displayName="Table5" ref="A1:J10" totalsRowShown="0">
   <autoFilter ref="A1:J10" xr:uid="{9B4D5B3D-846B-46CC-8CF1-243527D6D766}"/>
   <tableColumns count="10">
@@ -1873,7 +2302,7 @@
     <tableColumn id="5" xr3:uid="{917D8302-5D48-4C6E-A7A4-635B75B1AA68}" name="Color"/>
     <tableColumn id="6" xr3:uid="{2E1A7F23-7DD5-449A-B445-5CBCCBB12FEE}" name="Doors"/>
     <tableColumn id="7" xr3:uid="{3C31DEA5-29A1-41C7-B2D6-28A53CB066AA}" name="Trim"/>
-    <tableColumn id="8" xr3:uid="{AE52F333-84EB-4FC3-B679-EFBECEE0EA78}" name="Price" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{AE52F333-84EB-4FC3-B679-EFBECEE0EA78}" name="Price" dataDxfId="19"/>
     <tableColumn id="9" xr3:uid="{38688212-61AB-4FA4-8227-AE884E3E8008}" name="TopSpeed"/>
     <tableColumn id="10" xr3:uid="{F6DAC99F-5DA9-40D8-BB2F-C8A4FBFF8B8C}" name="OwnerId (FK)"/>
   </tableColumns>
@@ -1881,14 +2310,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BA013D20-4ABB-4616-B740-A9064E0348D7}" name="Table7" displayName="Table7" ref="A1:G10" totalsRowShown="0">
-  <autoFilter ref="A1:G10" xr:uid="{BA013D20-4ABB-4616-B740-A9064E0348D7}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8C7337AD-37D6-426E-94AA-9C158074F7C1}" name="SamuraiId"/>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BA013D20-4ABB-4616-B740-A9064E0348D7}" name="Table7" displayName="Table7" ref="A1:F10" totalsRowShown="0">
+  <autoFilter ref="A1:F10" xr:uid="{BA013D20-4ABB-4616-B740-A9064E0348D7}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8C7337AD-37D6-426E-94AA-9C158074F7C1}" name="SamuraiId(PK)"/>
     <tableColumn id="2" xr3:uid="{05661A05-493F-480C-BBEE-526CB04CC277}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{6326A3B7-C70A-47C3-A542-2F57039D6F18}" name="Weapon"/>
-    <tableColumn id="4" xr3:uid="{E5D7AE4D-A561-4D78-A256-54D6C73A60DC}" name="Armor"/>
+    <tableColumn id="4" xr3:uid="{E5D7AE4D-A561-4D78-A256-54D6C73A60DC}" name="Armor(FK)"/>
     <tableColumn id="5" xr3:uid="{07FCF174-67DA-408A-8651-C19D66CDE72B}" name="Mask"/>
     <tableColumn id="6" xr3:uid="{C6E51DB9-950A-4D4D-AAE7-D507C31029BF}" name="FollowsCode"/>
     <tableColumn id="7" xr3:uid="{C9E10016-83F6-45D8-B672-853CC7CD68F5}" name="SkillLevel"/>
@@ -1897,7 +2325,55 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{6C958ECC-5B48-4961-98C9-071E96F65BCB}" name="Table21" displayName="Table21" ref="A14:B16" totalsRowShown="0">
+  <autoFilter ref="A14:B16" xr:uid="{6C958ECC-5B48-4961-98C9-071E96F65BCB}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6A94BE5D-0C7D-4998-9E7D-9E73E27159D5}" name="WeaponId(PK)"/>
+    <tableColumn id="2" xr3:uid="{522E0BC1-563B-4AAD-BA22-69F5255875A5}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{4FE2160D-17E9-4125-850A-E5139783DA41}" name="Table22" displayName="Table22" ref="D14:E23" totalsRowShown="0">
+  <autoFilter ref="D14:E23" xr:uid="{4FE2160D-17E9-4125-850A-E5139783DA41}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{ACAAC582-15BC-4CDF-B322-F450E6871375}" name="SamuraiId(FK)" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{353263EE-1D81-46FA-8A1E-375ADFFD0B0B}" name="WeaponId(FK)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{16C1CB76-8CBB-40F3-8FB8-8A3D43B39CDC}" name="Table14" displayName="Table14" ref="A12:F20" totalsRowShown="0">
+  <autoFilter ref="A12:F20" xr:uid="{16C1CB76-8CBB-40F3-8FB8-8A3D43B39CDC}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{3C610158-F167-4CF0-9053-FB7C3A750B8E}" name="ShippingNumber(PK)"/>
+    <tableColumn id="2" xr3:uid="{6BD81B29-B8FB-4636-B400-EC6904F7B44E}" name="Destination" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{58151FA3-8AE0-4C40-A07F-64404B72B9AB}" name="LabelCreated" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{0CB887CD-B811-4C4D-B488-32B039756D05}" name="LastHandled" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{0B90C77E-161C-403F-96C6-B388D258E7B7}" name="Handler" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{E79E2D7F-DB8E-4E11-A658-97018C7F1EE0}" name="ProductId(FK)" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3224F6CB-249F-405E-B6C4-8D439ACA89C8}" name="Table23" displayName="Table23" ref="G14:H17" totalsRowShown="0">
+  <autoFilter ref="G14:H17" xr:uid="{3224F6CB-249F-405E-B6C4-8D439ACA89C8}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{04C197B4-A53C-4AE6-8C86-280D2ACE8F85}" name="ArmorId(PK)"/>
+    <tableColumn id="2" xr3:uid="{C12DC4C7-4B66-4E28-8C81-B5BFE9248382}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9A0FC7FA-1CB9-4069-8775-D0AE3643B0BD}" name="Table9" displayName="Table9" ref="A1:B21" totalsRowShown="0">
   <autoFilter ref="A1:B21" xr:uid="{9A0FC7FA-1CB9-4069-8775-D0AE3643B0BD}"/>
   <tableColumns count="2">
@@ -1908,15 +2384,14 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{93F42453-B6D9-40DA-ACF2-6737EC565292}" name="Table8" displayName="Table8" ref="A1:G6" totalsRowShown="0">
-  <autoFilter ref="A1:G6" xr:uid="{93F42453-B6D9-40DA-ACF2-6737EC565292}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D9268735-A887-445E-A97A-6BF04B4C397A}" name="BattleId"/>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{93F42453-B6D9-40DA-ACF2-6737EC565292}" name="Table8" displayName="Table8" ref="A1:F6" totalsRowShown="0">
+  <autoFilter ref="A1:F6" xr:uid="{93F42453-B6D9-40DA-ACF2-6737EC565292}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{D9268735-A887-445E-A97A-6BF04B4C397A}" name="BattleId(PK)"/>
     <tableColumn id="2" xr3:uid="{17E37DE7-9643-4CF2-B4B2-94537E73AABA}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{039C156A-475D-42D8-B852-940A07DA8C91}" name="Terrain"/>
-    <tableColumn id="4" xr3:uid="{EF24AB14-75E7-4DCD-939E-3E0249320437}" name="Location"/>
-    <tableColumn id="5" xr3:uid="{3AE997EA-2B3E-4A91-83BC-C26E8114C3BD}" name="Weather"/>
+    <tableColumn id="3" xr3:uid="{A51EE041-1ED5-464D-B597-CD4868B48922}" name="Location(FK)"/>
+    <tableColumn id="5" xr3:uid="{3AE997EA-2B3E-4A91-83BC-C26E8114C3BD}" name="Weather(FK)"/>
     <tableColumn id="6" xr3:uid="{55E25C6D-F88C-4354-A954-201C8B96F0C3}" name="Year"/>
     <tableColumn id="7" xr3:uid="{F477A209-DEF0-48B6-A461-04B4892C9E17}" name="NumberOfCommanders"/>
   </tableColumns>
@@ -1924,111 +2399,107 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C0A5FB02-0A02-40EE-AD8A-DB9B6C4B1594}" name="Table2" displayName="Table2" ref="A1:I6" totalsRowShown="0">
-  <autoFilter ref="A1:I6" xr:uid="{C0A5FB02-0A02-40EE-AD8A-DB9B6C4B1594}"/>
-  <tableColumns count="9">
-    <tableColumn id="11" xr3:uid="{94593037-8BD6-4DDF-95B4-2E447B1AC08E}" name="LocationId (PK)" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{E710B320-D3EE-417A-97E4-8BFF6658B181}" name="LocationName"/>
-    <tableColumn id="2" xr3:uid="{57ADD1CA-0C66-4E6D-BCC2-0B662EF20D13}" name="City"/>
-    <tableColumn id="3" xr3:uid="{32CE95FF-2B1A-4183-B68C-F33512A5EE91}" name="Country"/>
-    <tableColumn id="4" xr3:uid="{157FD42D-FFA0-4FA0-8901-C8C96F40317E}" name="Price" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{B7F7BBBA-D9C1-469A-9950-7CCF2EC5B539}" name="Airline"/>
-    <tableColumn id="6" xr3:uid="{65FA4FBA-ECC7-4D60-AA9B-39666DE62BE6}" name="Packages"/>
-    <tableColumn id="10" xr3:uid="{5C3DCE69-E03E-4474-849B-0F98760D25B6}" name="DepartureDate"/>
-    <tableColumn id="9" xr3:uid="{43CB51BE-33F7-4294-BB98-E4D297FD5A1F}" name="ReturnDate"/>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{72A5F40E-B648-40A7-8839-103B181F059A}" name="Table24" displayName="Table24" ref="A10:C15" totalsRowShown="0">
+  <autoFilter ref="A10:C15" xr:uid="{72A5F40E-B648-40A7-8839-103B181F059A}"/>
+  <tableColumns count="3">
+    <tableColumn id="4" xr3:uid="{00485BE3-7386-4094-8903-F8A9820176B1}" name="LandmarkId(PK)"/>
+    <tableColumn id="1" xr3:uid="{2162E61C-C40F-46F8-9249-449295DE04B9}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{67F3A99E-33D9-4E87-A0D6-582E27BA03E8}" name="Terrain"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{082686F0-0D97-4968-9676-6A5BE4102092}" name="Table25" displayName="Table25" ref="E10:F15" totalsRowShown="0">
+  <autoFilter ref="E10:F15" xr:uid="{082686F0-0D97-4968-9676-6A5BE4102092}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{98483AC8-F9BB-431A-ABCC-21EDFD61A889}" name="WeatherId"/>
+    <tableColumn id="2" xr3:uid="{CA29AB48-F4DA-407D-9FDA-9F8665850D74}" name="Pattern"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C0A5FB02-0A02-40EE-AD8A-DB9B6C4B1594}" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6" xr:uid="{C0A5FB02-0A02-40EE-AD8A-DB9B6C4B1594}"/>
+  <tableColumns count="3">
+    <tableColumn id="11" xr3:uid="{94593037-8BD6-4DDF-95B4-2E447B1AC08E}" name="LocationId (PK)" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{57ADD1CA-0C66-4E6D-BCC2-0B662EF20D13}" name="City"/>
+    <tableColumn id="3" xr3:uid="{32CE95FF-2B1A-4183-B68C-F33512A5EE91}" name="Country"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F78C787C-A553-4A7A-944D-B52DCDA2C501}" name="Table10" displayName="Table10" ref="A10:B15" totalsRowShown="0">
   <autoFilter ref="A10:B15" xr:uid="{F78C787C-A553-4A7A-944D-B52DCDA2C501}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9F945554-4336-41B3-B919-ECE6B8F0DC5E}" name="LanguageId"/>
+    <tableColumn id="1" xr3:uid="{9F945554-4336-41B3-B919-ECE6B8F0DC5E}" name="LanguageId(PK)"/>
     <tableColumn id="2" xr3:uid="{08E233F8-FF84-48E0-BDDD-1F6C080CE0AA}" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{27240001-C43E-4DA5-A2A7-174EA262335A}" name="Table11" displayName="Table11" ref="D10:E16" totalsRowShown="0">
   <autoFilter ref="D10:E16" xr:uid="{27240001-C43E-4DA5-A2A7-174EA262335A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EBF8334D-8514-44CA-8DC9-1A439513209D}" name="LocationId"/>
-    <tableColumn id="2" xr3:uid="{EC839AC5-5889-4F14-A648-3A9A7DD03971}" name="LanguageId"/>
+    <tableColumn id="1" xr3:uid="{EBF8334D-8514-44CA-8DC9-1A439513209D}" name="LocationId(FK)"/>
+    <tableColumn id="2" xr3:uid="{EC839AC5-5889-4F14-A648-3A9A7DD03971}" name="LanguageId(FK)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E8B06AB1-03A9-47AE-B8BF-BF5285966671}" name="Table12" displayName="Table12" ref="G10:H19" totalsRowShown="0">
   <autoFilter ref="G10:H19" xr:uid="{E8B06AB1-03A9-47AE-B8BF-BF5285966671}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1E1D8775-E7E2-4C04-A59A-629838277D32}" name="AttractionId"/>
+    <tableColumn id="1" xr3:uid="{1E1D8775-E7E2-4C04-A59A-629838277D32}" name="AttractionId(PK)"/>
     <tableColumn id="2" xr3:uid="{AB9588FB-39AA-484D-90F0-AA67E0C68372}" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{8B784324-716B-47A1-9880-EDB5DB949660}" name="Table13" displayName="Table13" ref="J10:K19" totalsRowShown="0">
   <autoFilter ref="J10:K19" xr:uid="{8B784324-716B-47A1-9880-EDB5DB949660}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{055C8F8C-A018-40F9-9BEA-CB34A59A6FEA}" name="LocationId"/>
-    <tableColumn id="2" xr3:uid="{473FDFDD-5A42-4E1F-BB20-32B3BB3D0343}" name="AttractionId"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9B1458FE-FA91-42BC-871C-630EB8E60412}" name="Table3" displayName="Table3" ref="A1:H9" totalsRowShown="0">
-  <autoFilter ref="A1:H9" xr:uid="{9B1458FE-FA91-42BC-871C-630EB8E60412}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{45BFCCB0-CFBB-4B57-8C28-AAC046F29FE2}" name="Title (PK)" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{D78FEB3F-9FBE-4352-BE7A-99B63B84046A}" name="ReleaseYear (PK)" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{D1A66C44-7E6F-4C4D-989B-89C81FC74AFD}" name="Genre" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{BBD5306B-D5DE-44D7-8410-6993F6B3F577}" name="Rating" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{952CD790-64DB-4FBD-BD46-21A5C343B1C9}" name="GrossProfit" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{1C33DB9A-FD12-47A9-AD86-D05FD166765F}" name="Cost" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{2E5F3783-24D8-4EA6-BAF7-DD66ACFB5965}" name="Runtime" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{572EC56E-E2A4-4FC3-9BB8-EC58E78E08A8}" name="ReviewScore"/>
+    <tableColumn id="1" xr3:uid="{055C8F8C-A018-40F9-9BEA-CB34A59A6FEA}" name="LocationId(FK)"/>
+    <tableColumn id="2" xr3:uid="{473FDFDD-5A42-4E1F-BB20-32B3BB3D0343}" name="AttractionId(FK)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{608619DC-1C9C-47A5-9711-DDF52ABEDA2F}" name="Table4" displayName="Table4" ref="A1:H8" totalsRowShown="0">
-  <autoFilter ref="A1:H8" xr:uid="{608619DC-1C9C-47A5-9711-DDF52ABEDA2F}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5A22A79B-FFD4-4DEB-9DBE-192986B98DE1}" name="PersonId (PK)"/>
-    <tableColumn id="2" xr3:uid="{FA34B470-FF1F-4B26-85CD-BCB40CADD0CC}" name="First"/>
-    <tableColumn id="3" xr3:uid="{146CC122-E9F9-442D-B20C-41BFF1898970}" name="Last"/>
-    <tableColumn id="4" xr3:uid="{1333BF0F-E4B6-4F51-B4B5-EA53C991A40F}" name="HairColor"/>
-    <tableColumn id="5" xr3:uid="{6AB9EFF3-157F-4350-BADB-555E7C3890A8}" name="Birthday" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{1D1456BC-3D5F-4581-9CFC-F74BFF30E53B}" name="BloodType"/>
-    <tableColumn id="7" xr3:uid="{B3996C23-B66E-4A7A-BE9F-1DC3E2A16BD0}" name="FirstLanguage"/>
-    <tableColumn id="8" xr3:uid="{5443F791-ACE7-4711-9651-CBBFDC16C2D7}" name="Job (FK)"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{129384F4-AF51-4960-9F3A-8DF978292172}" name="Table15" displayName="Table15" ref="A22:G27" totalsRowShown="0">
+  <autoFilter ref="A22:G27" xr:uid="{129384F4-AF51-4960-9F3A-8DF978292172}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8A40DF5D-E5E1-4632-8A8B-144F5D150A21}" name="ConfirmationNumber(PK)"/>
+    <tableColumn id="8" xr3:uid="{51877BE4-3A6D-4118-B073-A743F73DD37E}" name="Location(FK)" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{A54F08DA-0167-4146-88DD-10DBFBC76737}" name="AirlineId(FK)" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{DA73E77E-B63A-4036-995A-C93B479BC52A}" name="DepartureDate" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{B6576145-F14A-445A-9E5B-42CEF012F693}" name="ReturnDate" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{44362103-B69E-449D-8F1B-387EF3AE1E6C}" name="Package(FK)" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{30ADA43F-1D9D-4FA5-BA70-398466A6EF89}" name="Price" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B2843E5E-9CA7-4DEB-84C1-8D646C92F38C}" name="Table6" displayName="Table6" ref="A1:E7" totalsRowShown="0">
-  <autoFilter ref="A1:E7" xr:uid="{B2843E5E-9CA7-4DEB-84C1-8D646C92F38C}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E5CDF23F-8C1B-4148-9AEA-983FEA37C18D}" name="JobId (PK)"/>
-    <tableColumn id="2" xr3:uid="{9D7E6A9E-2E69-451B-A0FA-E94F9C3676DC}" name="Title"/>
-    <tableColumn id="3" xr3:uid="{FE0B5BBD-EF9F-4EB4-938A-BFA2D095CA92}" name="Company"/>
-    <tableColumn id="4" xr3:uid="{305ACE71-C1F4-4890-B6D6-E6F3B884C79B}" name="Salary"/>
-    <tableColumn id="5" xr3:uid="{0337C2FC-F46F-48C4-93E6-0DD9851D869D}" name="Description"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{85F49C53-AA07-4C20-BB79-B2C346DACECF}" name="Table16" displayName="Table16" ref="I22:J27" totalsRowShown="0">
+  <autoFilter ref="I22:J27" xr:uid="{85F49C53-AA07-4C20-BB79-B2C346DACECF}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{67FEA2F1-E288-4C43-9C68-71BBFE314048}" name="AirlineId(PK)" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{D40A2518-5F0C-4058-BC88-9D04EF23EC30}" name="Name" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2332,44 +2803,36 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3263EF81-4390-4578-998A-BBD02B26968B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
     <col min="2" max="2" width="15.109375" customWidth="1"/>
     <col min="3" max="3" width="16.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.88671875" customWidth="1"/>
     <col min="5" max="5" width="17.5546875" customWidth="1"/>
     <col min="6" max="6" width="15.88671875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2380,19 +2843,13 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3">
-        <v>45050</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3">
-        <v>45051</v>
+      <c r="D2" s="12">
+        <v>21</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2403,20 +2860,12 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3">
-        <v>45048</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3">
-        <v>45049</v>
-      </c>
+      <c r="D3" s="12">
+        <v>43</v>
+      </c>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -2426,20 +2875,12 @@
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="3">
-        <v>45037</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="3">
-        <v>45038</v>
-      </c>
+      <c r="D4" s="12">
+        <v>14</v>
+      </c>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -2449,20 +2890,12 @@
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3">
-        <v>44928</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3">
-        <v>44929</v>
-      </c>
+      <c r="D5" s="12">
+        <v>63</v>
+      </c>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -2472,20 +2905,12 @@
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3">
-        <v>45048</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3">
-        <v>45049</v>
-      </c>
+      <c r="D6" s="12">
+        <v>114</v>
+      </c>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -2495,20 +2920,12 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3">
-        <v>45052</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3">
-        <v>45053</v>
-      </c>
+      <c r="D7" s="12">
+        <v>40</v>
+      </c>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -2518,20 +2935,12 @@
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3">
-        <v>45000</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="3">
-        <v>45001</v>
-      </c>
+      <c r="D8" s="12">
+        <v>12</v>
+      </c>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -2541,25 +2950,202 @@
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="12">
+        <v>32</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45050</v>
+      </c>
+      <c r="D13" s="3">
+        <v>45051</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45048</v>
+      </c>
+      <c r="D14" s="3">
+        <v>45049</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>241</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45037</v>
+      </c>
+      <c r="D15" s="3">
+        <v>45038</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="3">
+        <v>44928</v>
+      </c>
+      <c r="D16" s="3">
+        <v>44929</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>244</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45048</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45049</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45052</v>
+      </c>
+      <c r="D18" s="3">
+        <v>45053</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>246</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45000</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45001</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="C20" s="3">
         <v>45021</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="D20" s="3">
+        <v>45022</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="3">
-        <v>45022</v>
+      <c r="F20" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2567,30 +3153,32 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BE5CF9-079B-4CF1-B1EB-81C50973515F}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>
     <col min="7" max="7" width="19.44140625" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
     <col min="10" max="10" width="16.109375" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
@@ -2598,55 +3186,19 @@
       <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>36</v>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="5">
-        <v>1000000</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="3">
-        <v>45049</v>
-      </c>
-      <c r="I2" s="4">
-        <v>45053</v>
-      </c>
-      <c r="J2" t="s">
-        <v>245</v>
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2654,57 +3206,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="6">
-        <v>5000</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="3">
-        <v>45050</v>
-      </c>
-      <c r="I3" s="4">
-        <v>45050</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
+      <c r="B4" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="5">
-        <v>3500</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="3">
-        <v>45037</v>
-      </c>
-      <c r="I4" s="4">
-        <v>45041</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2712,97 +3228,64 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="6">
-        <v>4650</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="3">
-        <v>44986</v>
-      </c>
-      <c r="I5" s="4">
-        <v>44995</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>41</v>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="5">
-        <v>7634</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="3">
-        <v>45080</v>
-      </c>
-      <c r="I6" s="3">
-        <v>45083</v>
-      </c>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="D9" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K9" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D10" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="E10" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="G10" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="H10" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="J10" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="K10" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2810,7 +3293,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2822,7 +3305,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -2836,7 +3319,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2848,7 +3331,7 @@
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -2862,7 +3345,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2874,7 +3357,7 @@
         <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -2888,7 +3371,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -2900,7 +3383,7 @@
         <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -2914,7 +3397,7 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -2926,7 +3409,7 @@
         <v>5</v>
       </c>
       <c r="H15" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="J15">
         <v>2</v>
@@ -2946,7 +3429,7 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J16">
         <v>3</v>
@@ -2955,12 +3438,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G17">
         <v>7</v>
       </c>
       <c r="H17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J17">
         <v>4</v>
@@ -2969,12 +3452,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G18">
         <v>8</v>
       </c>
       <c r="H18" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="J18">
         <v>5</v>
@@ -2983,29 +3466,262 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G19">
         <v>9</v>
       </c>
       <c r="H19" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="J19">
         <v>5</v>
       </c>
       <c r="K19">
         <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>265</v>
+      </c>
+      <c r="C21" t="s">
+        <v>264</v>
+      </c>
+      <c r="F21" t="s">
+        <v>266</v>
+      </c>
+      <c r="I21" t="s">
+        <v>261</v>
+      </c>
+      <c r="L21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>256</v>
+      </c>
+      <c r="B22" t="s">
+        <v>263</v>
+      </c>
+      <c r="C22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>258</v>
+      </c>
+      <c r="G22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" t="s">
+        <v>260</v>
+      </c>
+      <c r="J22" t="s">
+        <v>182</v>
+      </c>
+      <c r="L22" t="s">
+        <v>262</v>
+      </c>
+      <c r="M22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>45049</v>
+      </c>
+      <c r="E23" s="4">
+        <v>45053</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="H23" t="s">
+        <v>259</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>45050</v>
+      </c>
+      <c r="E24" s="4">
+        <v>45050</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="6">
+        <v>5000</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L24" s="1">
+        <v>2</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>45037</v>
+      </c>
+      <c r="E25" s="4">
+        <v>45041</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3</v>
+      </c>
+      <c r="G25" s="5">
+        <v>3500</v>
+      </c>
+      <c r="I25" s="1">
+        <v>3</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25" s="1">
+        <v>3</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3">
+        <v>44986</v>
+      </c>
+      <c r="E26" s="4">
+        <v>44995</v>
+      </c>
+      <c r="F26" s="1">
+        <v>4</v>
+      </c>
+      <c r="G26" s="6">
+        <v>4650</v>
+      </c>
+      <c r="I26" s="1">
+        <v>4</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L26" s="1">
+        <v>4</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3">
+        <v>45080</v>
+      </c>
+      <c r="E27" s="3">
+        <v>45083</v>
+      </c>
+      <c r="F27" s="1">
+        <v>5</v>
+      </c>
+      <c r="G27" s="5">
+        <v>7634</v>
+      </c>
+      <c r="I27" s="1">
+        <v>5</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L27" s="1">
+        <v>5</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="5">
+  <tableParts count="8">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3013,15 +3729,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA875229-1D8C-42F5-8899-72F7DCF9AFE1}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
@@ -3030,44 +3746,44 @@
     <col min="7" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="H1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="B2" s="2">
         <v>2001</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E2" s="5">
         <v>104900000</v>
@@ -3081,19 +3797,22 @@
       <c r="H2">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2">
         <v>1984</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="E3" s="5">
         <v>39900000</v>
@@ -3108,18 +3827,18 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2">
         <v>2000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E4" s="5">
         <v>27700000</v>
@@ -3134,18 +3853,18 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2">
         <v>1994</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E5" s="5">
         <v>678226465</v>
@@ -3160,18 +3879,18 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B6" s="2">
         <v>1960</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E6" s="5">
         <v>5500000</v>
@@ -3186,18 +3905,18 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2">
         <v>2016</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E7" s="5">
         <v>782600000</v>
@@ -3212,18 +3931,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2">
         <v>2019</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E8" s="5">
         <v>449762638</v>
@@ -3238,18 +3957,18 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B9" s="2">
         <v>1995</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E9" s="5">
         <v>187436818</v>
@@ -3279,7 +3998,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3296,28 +4015,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" t="s">
-        <v>98</v>
-      </c>
       <c r="H1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3325,22 +4044,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E2" s="7">
         <v>33981</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -3351,22 +4070,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E3" s="7">
         <v>33067</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -3377,22 +4096,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E4" s="7">
         <v>20152</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -3403,22 +4122,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E5" s="7">
         <v>20154</v>
       </c>
       <c r="F5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -3429,22 +4148,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E6" s="7">
         <v>25394</v>
       </c>
       <c r="F6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -3455,22 +4174,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E7" s="7">
         <v>31310</v>
       </c>
       <c r="F7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -3481,22 +4200,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E8" s="7">
         <v>816612</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H8">
         <v>6</v>
@@ -3512,37 +4231,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99004A48-90A8-4102-9853-76FE50478868}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
     <col min="5" max="5" width="33.88671875" customWidth="1"/>
     <col min="6" max="6" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3550,7 +4266,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -3558,7 +4277,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3566,7 +4285,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3574,7 +4293,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -3582,7 +4301,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -3590,13 +4309,109 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>269</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" t="s">
+        <v>275</v>
+      </c>
+      <c r="E11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>270</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>272</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3607,7 +4422,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3626,60 +4441,60 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
         <v>108</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>109</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>110</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
         <v>111</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>112</v>
       </c>
-      <c r="G1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1" t="s">
-        <v>115</v>
-      </c>
       <c r="K1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D2">
         <v>1998</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F2">
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H2" s="8">
         <v>30000</v>
@@ -3693,25 +4508,25 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D3">
         <v>1973</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H3" s="8">
         <v>45000</v>
@@ -3722,25 +4537,25 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D4">
         <v>2023</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H4" s="8">
         <v>45000</v>
@@ -3754,25 +4569,25 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D5">
         <v>1973</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H5" s="8">
         <v>56900</v>
@@ -3786,25 +4601,25 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D6">
         <v>1962</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H6" s="8">
         <v>131500.79999999999</v>
@@ -3815,25 +4630,25 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D7">
         <v>1969</v>
       </c>
       <c r="E7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H7" s="8">
         <v>200000</v>
@@ -3847,25 +4662,25 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D8">
         <v>1981</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H8" s="8">
         <v>300000</v>
@@ -3879,25 +4694,25 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D9">
         <v>1990</v>
       </c>
       <c r="E9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H9" s="8">
         <v>80000</v>
@@ -3911,25 +4726,25 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D10">
         <v>1955</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H10" s="8">
         <v>250000</v>
@@ -3952,257 +4767,366 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846305AF-C9AB-4320-9AD1-F739F97F29E8}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
     <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
     <col min="5" max="5" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="7" max="8" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" t="s">
         <v>184</v>
       </c>
-      <c r="B1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" t="s">
-        <v>205</v>
+        <v>192</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>205</v>
       </c>
-      <c r="D3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E3" t="s">
-        <v>213</v>
-      </c>
-      <c r="F3" t="b">
+      <c r="E3" t="b">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="F3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C4" t="s">
-        <v>205</v>
+        <v>194</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
-      </c>
-      <c r="E4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4">
+        <v>168</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" t="s">
-        <v>205</v>
+        <v>195</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5">
+        <v>168</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C6" t="s">
-        <v>205</v>
+        <v>196</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>209</v>
-      </c>
-      <c r="E6" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" t="b">
+        <v>168</v>
+      </c>
+      <c r="E6" t="b">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="F6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" t="s">
-        <v>205</v>
+        <v>198</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E7" t="s">
-        <v>212</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7">
+        <v>204</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C8" t="s">
-        <v>205</v>
+        <v>199</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>209</v>
-      </c>
-      <c r="E8" t="s">
-        <v>212</v>
-      </c>
-      <c r="F8" t="b">
+        <v>204</v>
+      </c>
+      <c r="E8" t="b">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C9" t="s">
-        <v>205</v>
+        <v>206</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>211</v>
-      </c>
-      <c r="E9" t="s">
-        <v>212</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9">
+        <v>204</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C10" t="s">
-        <v>205</v>
+        <v>200</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
-      </c>
-      <c r="E10" t="s">
-        <v>171</v>
-      </c>
-      <c r="F10" t="b">
+        <v>168</v>
+      </c>
+      <c r="E10" t="b">
         <v>0</v>
       </c>
-      <c r="G10">
+      <c r="F10">
         <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D13" t="s">
+        <v>279</v>
+      </c>
+      <c r="G13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G14" t="s">
+        <v>287</v>
+      </c>
+      <c r="H14" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>278</v>
+      </c>
+      <c r="D16" s="10">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D17" s="9">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D18" s="10">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D19" s="9">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D20" s="10">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D21" s="9">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D22" s="10">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="9">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4224,13 +5148,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -4241,7 +5165,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -4406,15 +5330,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0068CC6-62E7-4DE7-934F-2E8D1246E13A}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
     <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.88671875" customWidth="1"/>
@@ -4423,148 +5347,242 @@
     <col min="7" max="7" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>288</v>
       </c>
       <c r="B1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C1" t="s">
-        <v>192</v>
+        <v>263</v>
       </c>
       <c r="D1" t="s">
-        <v>193</v>
+        <v>293</v>
       </c>
       <c r="E1" t="s">
-        <v>194</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E2" t="s">
-        <v>217</v>
+        <v>207</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1995</v>
       </c>
       <c r="F2">
-        <v>1995</v>
-      </c>
-      <c r="G2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" t="s">
-        <v>224</v>
-      </c>
-      <c r="E3" t="s">
-        <v>225</v>
+        <v>211</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2000</v>
       </c>
       <c r="F3">
-        <v>2000</v>
-      </c>
-      <c r="G3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D4" t="s">
-        <v>221</v>
-      </c>
-      <c r="E4" t="s">
-        <v>222</v>
+        <v>212</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1995</v>
       </c>
       <c r="F4">
-        <v>1995</v>
-      </c>
-      <c r="G4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C5" t="s">
-        <v>227</v>
-      </c>
-      <c r="D5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E5" t="s">
-        <v>233</v>
+        <v>218</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>1977</v>
       </c>
       <c r="F5">
-        <v>1977</v>
-      </c>
-      <c r="G5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D6" t="s">
-        <v>230</v>
-      </c>
-      <c r="E6" t="s">
-        <v>231</v>
+        <v>220</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>2023</v>
       </c>
       <c r="F6">
-        <v>2023</v>
-      </c>
-      <c r="G6">
         <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" t="s">
+        <v>208</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" t="s">
+        <v>215</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C13" t="s">
+        <v>226</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" t="s">
+        <v>219</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>